<commit_message>
November 2015 data added
Not sure why, but I searched the council data website this morning and
the November 2015 data was there. I'm fairly sure it wasn't previously,
but the published date is well in the past, maybe I missed something.
</commit_message>
<xml_diff>
--- a/Data Quality.xlsx
+++ b/Data Quality.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="34">
   <si>
     <t>Month</t>
   </si>
@@ -122,6 +122,15 @@
   </si>
   <si>
     <t>Second line is dodgy, missing data?</t>
+  </si>
+  <si>
+    <t>… found the data, not sure why I didn't find it before</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://data.sheffield.gov.uk/Economy/November-2015-Monthly-Payments-To-Suppliers-Over-2/5iu7-7wgq/data</t>
   </si>
 </sst>
 </file>
@@ -132,7 +141,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +181,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -224,14 +241,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -267,11 +285,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -585,11 +605,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F80" sqref="F80"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,7 +620,7 @@
     <col min="6" max="6" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -616,8 +636,11 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>40544</v>
       </c>
@@ -637,7 +660,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>40575</v>
       </c>
@@ -649,7 +672,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>40603</v>
       </c>
@@ -661,7 +684,7 @@
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>40634</v>
       </c>
@@ -673,7 +696,7 @@
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>40664</v>
       </c>
@@ -685,7 +708,7 @@
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>40695</v>
       </c>
@@ -697,7 +720,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>40725</v>
       </c>
@@ -709,7 +732,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>40756</v>
       </c>
@@ -721,7 +744,7 @@
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>40787</v>
       </c>
@@ -733,7 +756,7 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>40817</v>
       </c>
@@ -745,7 +768,7 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>40848</v>
       </c>
@@ -757,7 +780,7 @@
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>40878</v>
       </c>
@@ -769,7 +792,7 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>40909</v>
       </c>
@@ -781,7 +804,7 @@
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>40940</v>
       </c>
@@ -793,7 +816,7 @@
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>40969</v>
       </c>
@@ -1189,7 +1212,7 @@
       <c r="E48" s="13"/>
       <c r="F48" s="13"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>41974</v>
       </c>
@@ -1201,7 +1224,7 @@
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>42005</v>
       </c>
@@ -1213,7 +1236,7 @@
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>42036</v>
       </c>
@@ -1225,7 +1248,7 @@
       <c r="E51" s="13"/>
       <c r="F51" s="13"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>42064</v>
       </c>
@@ -1237,7 +1260,7 @@
       <c r="E52" s="13"/>
       <c r="F52" s="13"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>42095</v>
       </c>
@@ -1249,7 +1272,7 @@
       <c r="E53" s="13"/>
       <c r="F53" s="13"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>42125</v>
       </c>
@@ -1261,7 +1284,7 @@
       <c r="E54" s="13"/>
       <c r="F54" s="13"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>42156</v>
       </c>
@@ -1273,7 +1296,7 @@
       <c r="E55" s="13"/>
       <c r="F55" s="13"/>
     </row>
-    <row r="56" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>42186</v>
       </c>
@@ -1291,7 +1314,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>42217</v>
       </c>
@@ -1303,7 +1326,7 @@
       <c r="E57" s="16"/>
       <c r="F57" s="13"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>42248</v>
       </c>
@@ -1320,7 +1343,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>42278</v>
       </c>
@@ -1337,19 +1360,27 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>42309</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C60" s="4"/>
-      <c r="E60" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B60" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" s="4">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60" t="s">
+        <v>31</v>
+      </c>
+      <c r="G60" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>42339</v>
       </c>
@@ -1366,7 +1397,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>42370</v>
       </c>
@@ -1383,7 +1414,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>42401</v>
       </c>
@@ -1400,7 +1431,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>42430</v>
       </c>
@@ -1729,6 +1760,9 @@
     <mergeCell ref="D56:D57"/>
     <mergeCell ref="D2:D55"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G60" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
April 2016 data added
Not sure why, but I searched the council data website this morning and
the April 2016 data was there. I'm fairly sure it wasn't previously,
but the published date is well in the past, maybe I missed something.
</commit_message>
<xml_diff>
--- a/Data Quality.xlsx
+++ b/Data Quality.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="35">
   <si>
     <t>Month</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>https://data.sheffield.gov.uk/Economy/November-2015-Monthly-Payments-To-Suppliers-Over-2/5iu7-7wgq/data</t>
+  </si>
+  <si>
+    <t>https://data.sheffield.gov.uk/Economy/April-2016-Monthly-Payments-To-Suppliers-Over-250-/rz5p-hfyt</t>
   </si>
 </sst>
 </file>
@@ -609,7 +612,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
+      <selection pane="bottomLeft" activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1448,19 +1451,27 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>42461</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C65" s="4"/>
-      <c r="E65" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B65" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="4">
+        <v>8</v>
+      </c>
+      <c r="D65" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65" t="s">
+        <v>31</v>
+      </c>
+      <c r="G65" s="19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>42491</v>
       </c>
@@ -1478,7 +1489,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>42522</v>
       </c>
@@ -1498,7 +1509,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>42552</v>
       </c>
@@ -1510,7 +1521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>42583</v>
       </c>
@@ -1522,7 +1533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>42614</v>
       </c>
@@ -1539,7 +1550,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>42644</v>
       </c>
@@ -1551,7 +1562,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>42675</v>
       </c>
@@ -1568,7 +1579,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>42705</v>
       </c>
@@ -1580,7 +1591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>42736</v>
       </c>
@@ -1597,7 +1608,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>42767</v>
       </c>
@@ -1609,7 +1620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>42795</v>
       </c>
@@ -1626,7 +1637,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>42826</v>
       </c>
@@ -1638,7 +1649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>42856</v>
       </c>
@@ -1650,7 +1661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>42887</v>
       </c>
@@ -1667,7 +1678,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>42917</v>
       </c>
@@ -1762,6 +1773,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G60" r:id="rId1"/>
+    <hyperlink ref="G65" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
July 2016 data added
Not sure why, but I searched the council data website this morning and
the July 2016 data was there. I'm fairly sure it wasn't previously,
but the published date is well in the past, maybe I missed something.
</commit_message>
<xml_diff>
--- a/Data Quality.xlsx
+++ b/Data Quality.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="36">
   <si>
     <t>Month</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>https://data.sheffield.gov.uk/Economy/April-2016-Monthly-Payments-To-Suppliers-Over-250-/rz5p-hfyt</t>
+  </si>
+  <si>
+    <t>https://data.sheffield.gov.uk/Economy/July-2016-Payments-To-Suppliers-Over-250-In-Value/3ta3-c3bu</t>
   </si>
 </sst>
 </file>
@@ -612,7 +615,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B65" sqref="B65"/>
+      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1513,12 +1516,20 @@
       <c r="A68" s="1">
         <v>42552</v>
       </c>
-      <c r="B68" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C68" s="4"/>
-      <c r="E68" s="3" t="s">
-        <v>4</v>
+      <c r="B68" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" s="4">
+        <v>8</v>
+      </c>
+      <c r="D68" t="s">
+        <v>13</v>
+      </c>
+      <c r="F68" t="s">
+        <v>31</v>
+      </c>
+      <c r="G68" s="19" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -1774,6 +1785,7 @@
   <hyperlinks>
     <hyperlink ref="G60" r:id="rId1"/>
     <hyperlink ref="G65" r:id="rId2"/>
+    <hyperlink ref="G68" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
August 2016 data added
Not sure why, but I searched the council data website this morning and
the August 2016 data was there. I'm fairly sure it wasn't previously,
but the published date is well in the past, maybe I missed something.
</commit_message>
<xml_diff>
--- a/Data Quality.xlsx
+++ b/Data Quality.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattt_000\Downloads\sheffield spend data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattt_000\Documents\GitHub\Sheffield-Spending-Data-Cleanup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="37">
   <si>
     <t>Month</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>https://data.sheffield.gov.uk/Economy/July-2016-Payments-To-Suppliers-Over-250-In-Value/3ta3-c3bu</t>
+  </si>
+  <si>
+    <t>https://data.sheffield.gov.uk/Economy/August-2016-Payments-To-Suppliers-Over-250-In-Valu/ffa2-kzhk</t>
   </si>
 </sst>
 </file>
@@ -273,6 +276,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -291,7 +295,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -614,8 +617,8 @@
   <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,16 +656,16 @@
       <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="16">
         <v>8</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="14" t="s">
         <v>29</v>
       </c>
     </row>
@@ -673,10 +676,10 @@
       <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -685,10 +688,10 @@
       <c r="B4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -697,10 +700,10 @@
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -709,10 +712,10 @@
       <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -721,10 +724,10 @@
       <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -733,10 +736,10 @@
       <c r="B8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -745,10 +748,10 @@
       <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -757,10 +760,10 @@
       <c r="B10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -769,10 +772,10 @@
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -781,10 +784,10 @@
       <c r="B12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -793,10 +796,10 @@
       <c r="B13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -805,10 +808,10 @@
       <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -817,10 +820,10 @@
       <c r="B15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -829,10 +832,10 @@
       <c r="B16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -841,10 +844,10 @@
       <c r="B17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -853,10 +856,10 @@
       <c r="B18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -865,10 +868,10 @@
       <c r="B19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
@@ -877,10 +880,10 @@
       <c r="B20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -889,10 +892,10 @@
       <c r="B21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -901,10 +904,10 @@
       <c r="B22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
@@ -913,10 +916,10 @@
       <c r="B23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
@@ -925,10 +928,10 @@
       <c r="B24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
@@ -937,10 +940,10 @@
       <c r="B25" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
@@ -949,10 +952,10 @@
       <c r="B26" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
@@ -961,10 +964,10 @@
       <c r="B27" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -973,10 +976,10 @@
       <c r="B28" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
@@ -985,10 +988,10 @@
       <c r="B29" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
@@ -997,10 +1000,10 @@
       <c r="B30" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
@@ -1009,10 +1012,10 @@
       <c r="B31" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
@@ -1021,10 +1024,10 @@
       <c r="B32" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
@@ -1033,10 +1036,10 @@
       <c r="B33" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
@@ -1045,10 +1048,10 @@
       <c r="B34" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
@@ -1057,10 +1060,10 @@
       <c r="B35" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
@@ -1069,10 +1072,10 @@
       <c r="B36" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
@@ -1081,10 +1084,10 @@
       <c r="B37" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
@@ -1093,10 +1096,10 @@
       <c r="B38" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
@@ -1105,10 +1108,10 @@
       <c r="B39" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="15"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
@@ -1117,10 +1120,10 @@
       <c r="B40" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
@@ -1129,10 +1132,10 @@
       <c r="B41" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
@@ -1141,10 +1144,10 @@
       <c r="B42" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
@@ -1153,10 +1156,10 @@
       <c r="B43" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
@@ -1165,10 +1168,10 @@
       <c r="B44" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
@@ -1177,10 +1180,10 @@
       <c r="B45" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
@@ -1189,10 +1192,10 @@
       <c r="B46" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
@@ -1201,10 +1204,10 @@
       <c r="B47" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
@@ -1213,10 +1216,10 @@
       <c r="B48" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
@@ -1225,10 +1228,10 @@
       <c r="B49" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
@@ -1237,10 +1240,10 @@
       <c r="B50" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
@@ -1249,10 +1252,10 @@
       <c r="B51" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
@@ -1261,10 +1264,10 @@
       <c r="B52" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C52" s="15"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
@@ -1273,10 +1276,10 @@
       <c r="B53" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
@@ -1285,10 +1288,10 @@
       <c r="B54" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C54" s="15"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
@@ -1297,10 +1300,10 @@
       <c r="B55" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="15"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
     </row>
     <row r="56" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
@@ -1309,14 +1312,14 @@
       <c r="B56" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="14">
+      <c r="C56" s="15">
         <v>8</v>
       </c>
-      <c r="D56" s="17" t="s">
+      <c r="D56" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E56" s="16"/>
-      <c r="F56" s="13" t="s">
+      <c r="E56" s="17"/>
+      <c r="F56" s="14" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1327,10 +1330,10 @@
       <c r="B57" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="14"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="13"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="14"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
@@ -1382,7 +1385,7 @@
       <c r="F60" t="s">
         <v>31</v>
       </c>
-      <c r="G60" s="19" t="s">
+      <c r="G60" s="13" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1470,7 +1473,7 @@
       <c r="F65" t="s">
         <v>31</v>
       </c>
-      <c r="G65" s="19" t="s">
+      <c r="G65" s="13" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1528,7 +1531,7 @@
       <c r="F68" t="s">
         <v>31</v>
       </c>
-      <c r="G68" s="19" t="s">
+      <c r="G68" s="13" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1536,12 +1539,18 @@
       <c r="A69" s="1">
         <v>42583</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>4</v>
+      <c r="B69" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C69" s="4"/>
-      <c r="E69" s="3" t="s">
-        <v>4</v>
+      <c r="D69" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" t="s">
+        <v>31</v>
+      </c>
+      <c r="G69" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
October 2016 data added
Not sure why, but I searched the council data website this morning and
the October 2016 data was there. I'm fairly sure it wasn't previously,
but the published date is well in the past, maybe I missed something.
</commit_message>
<xml_diff>
--- a/Data Quality.xlsx
+++ b/Data Quality.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="38">
   <si>
     <t>Month</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>https://data.sheffield.gov.uk/Economy/August-2016-Payments-To-Suppliers-Over-250-In-Valu/ffa2-kzhk</t>
+  </si>
+  <si>
+    <t>https://data.sheffield.gov.uk/Economy/October-2016-Monthly-Payments-To-Suppliers-Over-25/it4i-3itb</t>
   </si>
 </sst>
 </file>
@@ -617,8 +620,8 @@
   <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B69" sqref="B69"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1542,7 +1545,9 @@
       <c r="B69" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C69" s="4"/>
+      <c r="C69" s="4">
+        <v>8</v>
+      </c>
       <c r="D69" t="s">
         <v>7</v>
       </c>
@@ -1574,12 +1579,20 @@
       <c r="A71" s="1">
         <v>42644</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C71" s="4"/>
-      <c r="E71" s="3" t="s">
-        <v>4</v>
+      <c r="B71" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" s="4">
+        <v>8</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F71" t="s">
+        <v>31</v>
+      </c>
+      <c r="G71" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
December 2016 data added
Not sure why, but I searched the council data website this morning and
the December 2016 data was there. I'm fairly sure it wasn't previously,
but the published date is well in the past, maybe I missed something.
</commit_message>
<xml_diff>
--- a/Data Quality.xlsx
+++ b/Data Quality.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="40">
   <si>
     <t>Month</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>https://data.sheffield.gov.uk/Economy/October-2016-Monthly-Payments-To-Suppliers-Over-25/it4i-3itb</t>
+  </si>
+  <si>
+    <t>https://data.sheffield.gov.uk/Economy/December-2016-Monthly-Payments-To-Suppliers-Over-2/94fv-9zuq</t>
+  </si>
+  <si>
+    <t>mm/dd/yyyy</t>
   </si>
 </sst>
 </file>
@@ -620,8 +626,8 @@
   <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D71" sqref="D71"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1616,12 +1622,20 @@
       <c r="A73" s="1">
         <v>42705</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C73" s="4"/>
-      <c r="E73" s="3" t="s">
-        <v>4</v>
+      <c r="B73" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" s="4">
+        <v>8</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F73" t="s">
+        <v>31</v>
+      </c>
+      <c r="G73" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
February 2017 data added
Not sure why, but I searched the council data website this morning and
the February 2016 data was there. I'm fairly sure it wasn't previously,
but the published date is well in the past, maybe I missed something.
</commit_message>
<xml_diff>
--- a/Data Quality.xlsx
+++ b/Data Quality.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="41">
   <si>
     <t>Month</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>mm/dd/yyyy</t>
+  </si>
+  <si>
+    <t>https://data.sheffield.gov.uk/Economy/February-2017-Monthly-Payments-To-Suppliers-Over-2/b482-xxa6</t>
   </si>
 </sst>
 </file>
@@ -626,8 +629,8 @@
   <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D73" sqref="D73"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1659,12 +1662,20 @@
       <c r="A75" s="1">
         <v>42767</v>
       </c>
-      <c r="B75" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C75" s="4"/>
-      <c r="E75" s="3" t="s">
-        <v>4</v>
+      <c r="B75" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C75" s="4">
+        <v>8</v>
+      </c>
+      <c r="D75" t="s">
+        <v>7</v>
+      </c>
+      <c r="F75" t="s">
+        <v>31</v>
+      </c>
+      <c r="G75" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
April 2017 data added
Not sure why, but I searched the council data website this morning and
the April 2017 data was there. I'm fairly sure it wasn't previously,
but the published date is well in the past, maybe I missed something.
OMG the date format! '05 April 2017', that's a new one.
</commit_message>
<xml_diff>
--- a/Data Quality.xlsx
+++ b/Data Quality.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="43">
   <si>
     <t>Month</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>https://data.sheffield.gov.uk/Economy/February-2017-Monthly-Payments-To-Suppliers-Over-2/b482-xxa6</t>
+  </si>
+  <si>
+    <t>https://data.sheffield.gov.uk/Economy/April-2017-Monthly-Payments-To-Suppliers-Over-250-/u8nz-6n3y</t>
+  </si>
+  <si>
+    <t>03 April 2017</t>
   </si>
 </sst>
 </file>
@@ -270,7 +276,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -307,6 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -629,8 +636,8 @@
   <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1699,12 +1706,20 @@
       <c r="A77" s="1">
         <v>42826</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C77" s="4"/>
-      <c r="E77" s="3" t="s">
-        <v>4</v>
+      <c r="B77" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" s="4">
+        <v>8</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F77" t="s">
+        <v>31</v>
+      </c>
+      <c r="G77" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
May 2017 data added
Not sure why, but I searched the council data website this morning and
the May 2017  data was there. I'm fairly sure it wasn't previously,
but the published date is well in the past, maybe I missed something.
</commit_message>
<xml_diff>
--- a/Data Quality.xlsx
+++ b/Data Quality.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="44">
   <si>
     <t>Month</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>03 April 2017</t>
+  </si>
+  <si>
+    <t>https://data.sheffield.gov.uk/Economy/May-2017-Monthly-Payments-To-Suppliers-Over-250-In/9z8i-qtxm</t>
   </si>
 </sst>
 </file>
@@ -295,6 +298,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -313,7 +317,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -637,7 +640,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D77" sqref="D77"/>
+      <selection pane="bottomLeft" activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -675,16 +678,16 @@
       <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="16">
-        <v>8</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="C2" s="17">
+        <v>8</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="15" t="s">
         <v>29</v>
       </c>
     </row>
@@ -695,10 +698,10 @@
       <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -707,10 +710,10 @@
       <c r="B4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -719,10 +722,10 @@
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -731,10 +734,10 @@
       <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -743,10 +746,10 @@
       <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -755,10 +758,10 @@
       <c r="B8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -767,10 +770,10 @@
       <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -779,10 +782,10 @@
       <c r="B10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -791,10 +794,10 @@
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -803,10 +806,10 @@
       <c r="B12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -815,10 +818,10 @@
       <c r="B13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -827,10 +830,10 @@
       <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -839,10 +842,10 @@
       <c r="B15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -851,10 +854,10 @@
       <c r="B16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -863,10 +866,10 @@
       <c r="B17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -875,10 +878,10 @@
       <c r="B18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -887,10 +890,10 @@
       <c r="B19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
@@ -899,10 +902,10 @@
       <c r="B20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -911,10 +914,10 @@
       <c r="B21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -923,10 +926,10 @@
       <c r="B22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
@@ -935,10 +938,10 @@
       <c r="B23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
@@ -947,10 +950,10 @@
       <c r="B24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
@@ -959,10 +962,10 @@
       <c r="B25" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
@@ -971,10 +974,10 @@
       <c r="B26" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
@@ -983,10 +986,10 @@
       <c r="B27" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -995,10 +998,10 @@
       <c r="B28" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
@@ -1007,10 +1010,10 @@
       <c r="B29" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
@@ -1019,10 +1022,10 @@
       <c r="B30" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
@@ -1031,10 +1034,10 @@
       <c r="B31" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
@@ -1043,10 +1046,10 @@
       <c r="B32" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
@@ -1055,10 +1058,10 @@
       <c r="B33" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
@@ -1067,10 +1070,10 @@
       <c r="B34" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
@@ -1079,10 +1082,10 @@
       <c r="B35" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
@@ -1091,10 +1094,10 @@
       <c r="B36" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
@@ -1103,10 +1106,10 @@
       <c r="B37" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
@@ -1115,10 +1118,10 @@
       <c r="B38" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
@@ -1127,10 +1130,10 @@
       <c r="B39" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
@@ -1139,10 +1142,10 @@
       <c r="B40" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="16"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
@@ -1151,10 +1154,10 @@
       <c r="B41" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
@@ -1163,10 +1166,10 @@
       <c r="B42" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="16"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
@@ -1175,10 +1178,10 @@
       <c r="B43" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
@@ -1187,10 +1190,10 @@
       <c r="B44" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
@@ -1199,10 +1202,10 @@
       <c r="B45" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="16"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
@@ -1211,10 +1214,10 @@
       <c r="B46" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="16"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
@@ -1223,10 +1226,10 @@
       <c r="B47" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
@@ -1235,10 +1238,10 @@
       <c r="B48" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="16"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
@@ -1247,10 +1250,10 @@
       <c r="B49" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C49" s="16"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
@@ -1259,10 +1262,10 @@
       <c r="B50" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C50" s="16"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
@@ -1271,10 +1274,10 @@
       <c r="B51" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="16"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
@@ -1283,10 +1286,10 @@
       <c r="B52" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C52" s="16"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
@@ -1295,10 +1298,10 @@
       <c r="B53" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="16"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
@@ -1307,10 +1310,10 @@
       <c r="B54" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C54" s="16"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
@@ -1319,10 +1322,10 @@
       <c r="B55" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="16"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
     </row>
     <row r="56" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
@@ -1331,14 +1334,14 @@
       <c r="B56" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="15">
-        <v>8</v>
-      </c>
-      <c r="D56" s="18" t="s">
+      <c r="C56" s="16">
+        <v>8</v>
+      </c>
+      <c r="D56" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E56" s="17"/>
-      <c r="F56" s="14" t="s">
+      <c r="E56" s="18"/>
+      <c r="F56" s="15" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1349,10 +1352,10 @@
       <c r="B57" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="15"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="14"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="15"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
@@ -1712,7 +1715,7 @@
       <c r="C77" s="4">
         <v>8</v>
       </c>
-      <c r="D77" s="20" t="s">
+      <c r="D77" s="14" t="s">
         <v>42</v>
       </c>
       <c r="F77" t="s">
@@ -1726,12 +1729,20 @@
       <c r="A78" s="1">
         <v>42856</v>
       </c>
-      <c r="B78" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C78" s="4"/>
-      <c r="E78" s="3" t="s">
-        <v>4</v>
+      <c r="B78" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" s="4">
+        <v>8</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F78" t="s">
+        <v>31</v>
+      </c>
+      <c r="G78" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>